<commit_message>
Working version using CLK_IN, requires further testing.
</commit_message>
<xml_diff>
--- a/adas1000-4-registers.xlsx
+++ b/adas1000-4-registers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Musa Mahmood\Dropbox (GaTech)\NRF\nRF5_SDK_13.1.0\examples\_my_projects\nRF52-ADAS1000-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6B16A9-F66A-4353-9BD5-E3D6F62A3B0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B63E0A-DBA2-4AB0-8296-4C336ACB2356}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,7 +289,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +326,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +357,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -375,7 +402,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -389,7 +416,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -677,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,57 +836,57 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="11">
         <v>58</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="9" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(K2+2*J2+4*I2+8*H2+16*G2+32*F2+64*E2+128*D2,2),"00")</f>
         <v>0xE0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="str">
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(T2+2*S2+4*R2+8*Q2+16*P2+32*O2+64*N2+128*M2,2),"00")</f>
         <v>0x00</v>
       </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="7">
         <v>0</v>
       </c>
       <c r="S2" s="2">
@@ -854,30 +895,30 @@
       <c r="T2" s="2">
         <v>0</v>
       </c>
-      <c r="U2" t="str">
+      <c r="U2" s="9" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(AC2+2*AB2+4*AA2+8*Z2+16*Y2+32*X2+64*W2+128*V2,2),"00")</f>
-        <v>0x00</v>
+        <v>0xE6</v>
       </c>
       <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W2" s="7">
+        <v>1</v>
+      </c>
+      <c r="X2" s="7">
+        <v>1</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="7">
         <v>0</v>
       </c>
       <c r="AA2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2" s="2">
         <v>0</v>
@@ -890,7 +931,7 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="11">
         <v>59</v>
       </c>
       <c r="C3" t="str">
@@ -985,7 +1026,7 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="11">
         <v>60</v>
       </c>
       <c r="C4" t="str">
@@ -1076,11 +1117,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="11">
         <v>61</v>
       </c>
       <c r="C5" t="str">
@@ -1171,14 +1212,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="11">
         <v>62</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0xE0</v>
       </c>
@@ -1191,38 +1232,38 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" t="str">
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>0x00</v>
       </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" s="2">
@@ -1234,9 +1275,9 @@
       <c r="T6" s="2">
         <v>0</v>
       </c>
-      <c r="U6" t="str">
+      <c r="U6" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>0x00</v>
+        <v>0x0A</v>
       </c>
       <c r="V6" s="2">
         <v>0</v>
@@ -1250,27 +1291,27 @@
       <c r="Y6" s="2">
         <v>0</v>
       </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="2">
+      <c r="Z6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="7">
         <v>0</v>
       </c>
       <c r="AD6" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="11">
         <v>63</v>
       </c>
       <c r="C7" t="str">
@@ -1365,7 +1406,7 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="11">
         <v>64</v>
       </c>
       <c r="C8" t="str">
@@ -1460,7 +1501,7 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="11">
         <v>64</v>
       </c>
       <c r="C9" t="str">
@@ -1555,7 +1596,7 @@
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="12">
         <v>65</v>
       </c>
       <c r="C10" s="6" t="str">
@@ -1647,46 +1688,46 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="12">
         <v>66</v>
       </c>
-      <c r="C11" s="6" t="str">
+      <c r="C11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0x00</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
+        <v>0x1F</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>0x00</v>
+        <v>0x96</v>
       </c>
       <c r="M11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="4">
         <v>0</v>
@@ -1695,21 +1736,21 @@
         <v>0</v>
       </c>
       <c r="P11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="4">
         <v>0</v>
       </c>
       <c r="R11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="4">
         <v>0</v>
       </c>
-      <c r="U11" s="6" t="str">
+      <c r="U11" s="10" t="str">
         <f t="shared" si="2"/>
         <v>0x00</v>
       </c>
@@ -1745,7 +1786,7 @@
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="12">
         <v>67</v>
       </c>
       <c r="C12" s="6" t="str">
@@ -1840,7 +1881,7 @@
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="12">
         <v>67</v>
       </c>
       <c r="C13" s="6" t="str">
@@ -1935,7 +1976,7 @@
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="13">
         <v>67</v>
       </c>
       <c r="C14" s="5" t="str">
@@ -2030,7 +2071,7 @@
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="13">
         <v>68</v>
       </c>
       <c r="C15" s="5" t="str">
@@ -2125,7 +2166,7 @@
       <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="13">
         <v>68</v>
       </c>
       <c r="C16" s="5" t="str">
@@ -2220,7 +2261,7 @@
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="13">
         <v>68</v>
       </c>
       <c r="C17" s="5" t="str">
@@ -2315,7 +2356,7 @@
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="12">
         <v>68</v>
       </c>
       <c r="C18" s="6" t="str">
@@ -2410,7 +2451,7 @@
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="12">
         <v>68</v>
       </c>
       <c r="C19" s="6" t="str">
@@ -2505,7 +2546,7 @@
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="12">
         <v>69</v>
       </c>
       <c r="C20" t="str">
@@ -2600,7 +2641,7 @@
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="12">
         <v>69</v>
       </c>
       <c r="C21" t="str">
@@ -2695,7 +2736,7 @@
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="12">
         <v>69</v>
       </c>
       <c r="C22" t="str">
@@ -2790,7 +2831,7 @@
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="11">
         <v>70</v>
       </c>
       <c r="C23" t="str">
@@ -2885,7 +2926,7 @@
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="11">
         <v>70</v>
       </c>
       <c r="C24" t="str">
@@ -2980,7 +3021,7 @@
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="12">
         <v>71</v>
       </c>
       <c r="C25" t="str">
@@ -3075,7 +3116,7 @@
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="12">
         <v>71</v>
       </c>
       <c r="C26" t="str">
@@ -3170,7 +3211,7 @@
       <c r="A27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="12">
         <v>71</v>
       </c>
       <c r="C27" t="str">
@@ -3265,7 +3306,7 @@
       <c r="A28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="12">
         <v>71</v>
       </c>
       <c r="C28" t="str">
@@ -3360,7 +3401,7 @@
       <c r="A29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="12">
         <v>72</v>
       </c>
       <c r="C29" t="str">
@@ -3455,7 +3496,7 @@
       <c r="A30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="12">
         <v>72</v>
       </c>
       <c r="C30" t="str">
@@ -3550,7 +3591,7 @@
       <c r="A31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="12">
         <v>72</v>
       </c>
       <c r="C31" t="str">
@@ -3645,7 +3686,7 @@
       <c r="A32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="12">
         <v>72</v>
       </c>
       <c r="C32" t="str">
@@ -3740,7 +3781,7 @@
       <c r="A33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="12">
         <v>72</v>
       </c>
       <c r="C33" t="str">
@@ -3835,7 +3876,7 @@
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="12">
         <v>72</v>
       </c>
       <c r="C34" t="str">
@@ -3930,7 +3971,7 @@
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="11">
         <v>73</v>
       </c>
       <c r="C35" t="str">
@@ -4025,7 +4066,7 @@
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="11">
         <v>73</v>
       </c>
       <c r="C36" t="str">

</xml_diff>

<commit_message>
Working BLE Transfer, with test 3-lead ECG setup.
</commit_message>
<xml_diff>
--- a/adas1000-4-registers.xlsx
+++ b/adas1000-4-registers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Musa Mahmood\Dropbox (GaTech)\NRF\nRF5_SDK_13.1.0\examples\_my_projects\nRF52-ADAS1000-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (GaTech)\NRF\nRF5_SDK_13.1.0\examples\_my_projects\nRF52-ADAS1000-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B63E0A-DBA2-4AB0-8296-4C336ACB2356}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -283,13 +282,19 @@
   </si>
   <si>
     <t>LOAMRA</t>
+  </si>
+  <si>
+    <t>*** TEMPORARY SETUP FOR EXAMPLE ***</t>
+  </si>
+  <si>
+    <t>500 Hz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +346,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,8 +383,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -395,14 +412,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,12 +475,22 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -715,11 +767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +949,7 @@
       </c>
       <c r="U2" s="9" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(AC2+2*AB2+4*AA2+8*Z2+16*Y2+32*X2+64*W2+128*V2,2),"00")</f>
-        <v>0xE6</v>
+        <v>0xC6</v>
       </c>
       <c r="V2" s="2">
         <v>1</v>
@@ -906,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="X2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>
@@ -1592,7 +1644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1687,7 +1739,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1707,26 +1759,26 @@
       <c r="F11" s="8">
         <v>0</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>1</v>
       </c>
       <c r="L11" s="10" t="str">
         <f t="shared" si="1"/>
         <v>0x96</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>1</v>
       </c>
       <c r="N11" s="4">
@@ -1757,7 +1809,7 @@
       <c r="V11" s="4">
         <v>0</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11" s="8">
         <v>0</v>
       </c>
       <c r="X11" s="4">
@@ -1782,7 +1834,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -4162,7 +4214,116 @@
         <v>46</v>
       </c>
     </row>
+    <row r="39" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="12">
+        <v>66</v>
+      </c>
+      <c r="C40" s="10" t="str">
+        <f t="shared" ref="C40" si="9">"0x"&amp;TEXT(DEC2HEX(K40+2*J40+4*I40+8*H40+16*G40+32*F40+64*E40+128*D40,2),"00")</f>
+        <v>0x1F</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
+      <c r="L40" s="10" t="str">
+        <f t="shared" ref="L40" si="10">"0x"&amp;TEXT(DEC2HEX(T40+2*S40+4*R40+8*Q40+16*P40+32*O40+64*N40+128*M40,2),"00")</f>
+        <v>0xFE</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1</v>
+      </c>
+      <c r="N40" s="4">
+        <v>1</v>
+      </c>
+      <c r="O40" s="4">
+        <v>1</v>
+      </c>
+      <c r="P40" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>1</v>
+      </c>
+      <c r="R40" s="4">
+        <v>1</v>
+      </c>
+      <c r="S40" s="4">
+        <v>1</v>
+      </c>
+      <c r="T40" s="3">
+        <v>0</v>
+      </c>
+      <c r="U40" s="10" t="str">
+        <f t="shared" ref="U40" si="11">"0x"&amp;TEXT(DEC2HEX(AC40+2*AB40+4*AA40+8*Z40+16*Y40+32*X40+64*W40+128*V40,2),"00")</f>
+        <v>0x88</v>
+      </c>
+      <c r="V40" s="4">
+        <v>1</v>
+      </c>
+      <c r="W40" s="8">
+        <v>0</v>
+      </c>
+      <c r="X40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Z41" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA41" s="16"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Z41:AA41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated default settings to 31.25 Hz data. Added ability to alter default registers via BLE.
</commit_message>
<xml_diff>
--- a/adas1000-4-registers.xlsx
+++ b/adas1000-4-registers.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RespConfig01" sheetId="2" r:id="rId2"/>
     <sheet name="RespConfig02" sheetId="3" r:id="rId3"/>
+    <sheet name="Resp_500Hz" sheetId="4" r:id="rId4"/>
+    <sheet name="HRRR_500_2MSPS" sheetId="5" r:id="rId5"/>
+    <sheet name="HRRR_final_1MSPS_31.25" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="103">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -314,6 +317,33 @@
   </si>
   <si>
     <t>32-bit header:</t>
+  </si>
+  <si>
+    <t>Threshold = N × 2 × VREF/GAIN/2^16</t>
+  </si>
+  <si>
+    <t>0 = PACEAMPTH/2</t>
+  </si>
+  <si>
+    <t>0 = 0x00 = 0 V</t>
+  </si>
+  <si>
+    <t>−1 = 0xFF = −VREF/gain/2^16</t>
+  </si>
+  <si>
+    <t>1 = VREF/gain/2^16</t>
+  </si>
+  <si>
+    <t>N = N × VREF/gain/2^16</t>
+  </si>
+  <si>
+    <t>+1 = 0x01 = +VREF/gain/2^16</t>
+  </si>
+  <si>
+    <t>High power mode (temp)</t>
+  </si>
+  <si>
+    <t>THIS IS A SIGNED VALUE</t>
   </si>
 </sst>
 </file>
@@ -401,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,8 +481,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -648,6 +684,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -658,7 +805,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -781,6 +928,175 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4626,10 +4942,10 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="AA41" s="46" t="s">
+      <c r="AA41" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="AB41" s="46"/>
+      <c r="AB41" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4645,7 +4961,7 @@
   <dimension ref="A1:AD13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4661,36 +4977,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
+      <c r="U1" s="106"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="106"/>
+      <c r="Y1" s="106"/>
+      <c r="Z1" s="106"/>
+      <c r="AA1" s="106"/>
+      <c r="AB1" s="106"/>
     </row>
     <row r="2" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4886,7 +5202,7 @@
       </c>
       <c r="D4" s="22" t="str">
         <f t="shared" ref="D4:D7" si="0">"0x00"&amp;TEXT(DEC2HEX(L4+2*K4+4*J4+8*I4+16*H4+32*G4+64*F4+128*E4,2),"00")&amp;TEXT(DEC2HEX(T4+2*S4+4*R4+8*Q4+16*P4+32*O4+64*N4+128*M4,2),"00")&amp;TEXT(DEC2HEX(AB4+2*AA4+4*Z4+8*Y4+16*X4+32*W4+64*V4+128*U4,2),"00")</f>
-        <v>0x001FCE88</v>
+        <v>0x001F8E0B</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -4916,7 +5232,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="19">
         <v>0</v>
@@ -4937,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="8">
         <v>0</v>
@@ -4955,10 +5271,10 @@
         <v>0</v>
       </c>
       <c r="AA4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="s">
         <v>90</v>
@@ -5255,8 +5571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6168,12 +6484,12 @@
       </c>
     </row>
     <row r="16" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
       <c r="E16" s="4">
         <v>31</v>
       </c>
@@ -6389,4 +6705,2975 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="3.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="3" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3" style="47" customWidth="1"/>
+    <col min="15" max="18" width="3" style="47" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="47" customWidth="1"/>
+    <col min="20" max="20" width="3" style="47" customWidth="1"/>
+    <col min="21" max="28" width="3.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" style="47" customWidth="1"/>
+    <col min="31" max="31" width="25.28515625" style="47" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="48">
+        <v>23</v>
+      </c>
+      <c r="F1" s="48">
+        <v>22</v>
+      </c>
+      <c r="G1" s="48">
+        <v>21</v>
+      </c>
+      <c r="H1" s="48">
+        <v>20</v>
+      </c>
+      <c r="I1" s="48">
+        <v>19</v>
+      </c>
+      <c r="J1" s="48">
+        <v>18</v>
+      </c>
+      <c r="K1" s="48">
+        <v>17</v>
+      </c>
+      <c r="L1" s="49">
+        <v>16</v>
+      </c>
+      <c r="M1" s="54">
+        <v>15</v>
+      </c>
+      <c r="N1" s="48">
+        <v>14</v>
+      </c>
+      <c r="O1" s="48">
+        <v>13</v>
+      </c>
+      <c r="P1" s="48">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="48">
+        <v>11</v>
+      </c>
+      <c r="R1" s="48">
+        <v>10</v>
+      </c>
+      <c r="S1" s="48">
+        <v>9</v>
+      </c>
+      <c r="T1" s="49">
+        <v>8</v>
+      </c>
+      <c r="U1" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="11">
+        <v>62</v>
+      </c>
+      <c r="D2" s="75" t="str">
+        <f>"0x00"&amp;TEXT(DEC2HEX(L2+2*K2+4*J2+8*I2+16*H2+32*G2+64*F2+128*E2,2),"00")&amp;TEXT(DEC2HEX(T2+2*S2+4*R2+8*Q2+16*P2+32*O2+64*N2+128*M2,2),"00")&amp;TEXT(DEC2HEX(AB2+2*AA2+4*Z2+8*Y2+16*X2+32*W2+64*V2+128*U2,2),"00")</f>
+        <v>0x00A0000A</v>
+      </c>
+      <c r="E2" s="28">
+        <v>1</v>
+      </c>
+      <c r="F2" s="36">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34">
+        <v>1</v>
+      </c>
+      <c r="H2" s="30">
+        <v>0</v>
+      </c>
+      <c r="I2" s="50">
+        <v>0</v>
+      </c>
+      <c r="J2" s="50">
+        <v>0</v>
+      </c>
+      <c r="K2" s="50">
+        <v>0</v>
+      </c>
+      <c r="L2" s="51">
+        <v>0</v>
+      </c>
+      <c r="M2" s="55">
+        <v>0</v>
+      </c>
+      <c r="N2" s="27">
+        <v>0</v>
+      </c>
+      <c r="O2" s="28">
+        <v>0</v>
+      </c>
+      <c r="P2" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="50">
+        <v>0</v>
+      </c>
+      <c r="R2" s="50">
+        <v>0</v>
+      </c>
+      <c r="S2" s="48">
+        <v>0</v>
+      </c>
+      <c r="T2" s="56">
+        <v>0</v>
+      </c>
+      <c r="U2" s="54">
+        <v>0</v>
+      </c>
+      <c r="V2" s="48">
+        <v>0</v>
+      </c>
+      <c r="W2" s="48">
+        <v>0</v>
+      </c>
+      <c r="X2" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="62">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="62">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="62">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="64">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="12">
+        <v>66</v>
+      </c>
+      <c r="D3" s="75" t="str">
+        <f t="shared" ref="D3:D10" si="0">"0x00"&amp;TEXT(DEC2HEX(L3+2*K3+4*J3+8*I3+16*H3+32*G3+64*F3+128*E3,2),"00")&amp;TEXT(DEC2HEX(T3+2*S3+4*R3+8*Q3+16*P3+32*O3+64*N3+128*M3,2),"00")&amp;TEXT(DEC2HEX(AB3+2*AA3+4*Z3+8*Y3+16*X3+32*W3+64*V3+128*U3,2),"00")</f>
+        <v>0x001F8E08</v>
+      </c>
+      <c r="E3" s="72">
+        <v>0</v>
+      </c>
+      <c r="F3" s="37">
+        <v>0</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
+        <v>1</v>
+      </c>
+      <c r="I3" s="50">
+        <v>1</v>
+      </c>
+      <c r="J3" s="50">
+        <v>1</v>
+      </c>
+      <c r="K3" s="50">
+        <v>1</v>
+      </c>
+      <c r="L3" s="51">
+        <v>1</v>
+      </c>
+      <c r="M3" s="57">
+        <v>1</v>
+      </c>
+      <c r="N3" s="58">
+        <v>0</v>
+      </c>
+      <c r="O3" s="58">
+        <v>0</v>
+      </c>
+      <c r="P3" s="58">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="59">
+        <v>1</v>
+      </c>
+      <c r="R3" s="59">
+        <v>1</v>
+      </c>
+      <c r="S3" s="59">
+        <v>1</v>
+      </c>
+      <c r="T3" s="51">
+        <v>0</v>
+      </c>
+      <c r="U3" s="65">
+        <v>0</v>
+      </c>
+      <c r="V3" s="59">
+        <v>0</v>
+      </c>
+      <c r="W3" s="50">
+        <v>0</v>
+      </c>
+      <c r="X3" s="66">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="67">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="67">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="68">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="69">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="11">
+        <v>58</v>
+      </c>
+      <c r="D4" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00A004C6</v>
+      </c>
+      <c r="E4" s="73">
+        <v>1</v>
+      </c>
+      <c r="F4" s="37">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50">
+        <v>0</v>
+      </c>
+      <c r="J4" s="50">
+        <v>0</v>
+      </c>
+      <c r="K4" s="50">
+        <v>0</v>
+      </c>
+      <c r="L4" s="51">
+        <v>0</v>
+      </c>
+      <c r="M4" s="57">
+        <v>0</v>
+      </c>
+      <c r="N4" s="50">
+        <v>0</v>
+      </c>
+      <c r="O4" s="50">
+        <v>0</v>
+      </c>
+      <c r="P4" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="50">
+        <v>0</v>
+      </c>
+      <c r="R4" s="60">
+        <v>1</v>
+      </c>
+      <c r="S4" s="48">
+        <v>0</v>
+      </c>
+      <c r="T4" s="49">
+        <v>0</v>
+      </c>
+      <c r="U4" s="54">
+        <v>1</v>
+      </c>
+      <c r="V4" s="62">
+        <v>1</v>
+      </c>
+      <c r="W4" s="62">
+        <v>0</v>
+      </c>
+      <c r="X4" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="48">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="48">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="49">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="11">
+        <v>60</v>
+      </c>
+      <c r="D5" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00002019</v>
+      </c>
+      <c r="E5" s="74">
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="32">
+        <v>0</v>
+      </c>
+      <c r="H5" s="50">
+        <v>0</v>
+      </c>
+      <c r="I5" s="50">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50">
+        <v>0</v>
+      </c>
+      <c r="K5" s="50">
+        <v>0</v>
+      </c>
+      <c r="L5" s="49">
+        <v>0</v>
+      </c>
+      <c r="M5" s="54">
+        <v>0</v>
+      </c>
+      <c r="N5" s="48">
+        <v>0</v>
+      </c>
+      <c r="O5" s="58">
+        <v>1</v>
+      </c>
+      <c r="P5" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>0</v>
+      </c>
+      <c r="R5" s="25">
+        <v>0</v>
+      </c>
+      <c r="S5" s="25">
+        <v>0</v>
+      </c>
+      <c r="T5" s="61">
+        <v>0</v>
+      </c>
+      <c r="U5" s="70">
+        <v>0</v>
+      </c>
+      <c r="V5" s="48">
+        <v>0</v>
+      </c>
+      <c r="W5" s="48">
+        <v>0</v>
+      </c>
+      <c r="X5" s="33">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="38">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="11">
+        <v>61</v>
+      </c>
+      <c r="D6" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000E01</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="50">
+        <v>0</v>
+      </c>
+      <c r="G6" s="50">
+        <v>0</v>
+      </c>
+      <c r="H6" s="50">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50">
+        <v>0</v>
+      </c>
+      <c r="K6" s="50">
+        <v>0</v>
+      </c>
+      <c r="L6" s="51">
+        <v>0</v>
+      </c>
+      <c r="M6" s="57">
+        <v>0</v>
+      </c>
+      <c r="N6" s="50">
+        <v>0</v>
+      </c>
+      <c r="O6" s="50">
+        <v>0</v>
+      </c>
+      <c r="P6" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="62">
+        <v>1</v>
+      </c>
+      <c r="R6" s="62">
+        <v>1</v>
+      </c>
+      <c r="S6" s="62">
+        <v>1</v>
+      </c>
+      <c r="T6" s="44">
+        <v>0</v>
+      </c>
+      <c r="U6" s="44">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27">
+        <v>0</v>
+      </c>
+      <c r="W6" s="29">
+        <v>0</v>
+      </c>
+      <c r="X6" s="33">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="11">
+        <v>64</v>
+      </c>
+      <c r="D7" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0024242C</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0</v>
+      </c>
+      <c r="F7" s="48">
+        <v>0</v>
+      </c>
+      <c r="G7" s="48">
+        <v>1</v>
+      </c>
+      <c r="H7" s="48">
+        <v>0</v>
+      </c>
+      <c r="I7" s="48">
+        <v>0</v>
+      </c>
+      <c r="J7" s="48">
+        <v>1</v>
+      </c>
+      <c r="K7" s="48">
+        <v>0</v>
+      </c>
+      <c r="L7" s="49">
+        <v>0</v>
+      </c>
+      <c r="M7" s="48">
+        <v>0</v>
+      </c>
+      <c r="N7" s="48">
+        <v>0</v>
+      </c>
+      <c r="O7" s="48">
+        <v>1</v>
+      </c>
+      <c r="P7" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="48">
+        <v>0</v>
+      </c>
+      <c r="R7" s="48">
+        <v>1</v>
+      </c>
+      <c r="S7" s="48">
+        <v>0</v>
+      </c>
+      <c r="T7" s="49">
+        <v>0</v>
+      </c>
+      <c r="U7" s="62">
+        <v>0</v>
+      </c>
+      <c r="V7" s="62">
+        <v>0</v>
+      </c>
+      <c r="W7" s="62">
+        <v>1</v>
+      </c>
+      <c r="X7" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="62">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="62">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="64">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="13">
+        <v>68</v>
+      </c>
+      <c r="D8" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E8" s="52">
+        <v>0</v>
+      </c>
+      <c r="F8" s="52">
+        <v>0</v>
+      </c>
+      <c r="G8" s="52">
+        <v>0</v>
+      </c>
+      <c r="H8" s="52">
+        <v>0</v>
+      </c>
+      <c r="I8" s="52">
+        <v>0</v>
+      </c>
+      <c r="J8" s="52">
+        <v>0</v>
+      </c>
+      <c r="K8" s="52">
+        <v>0</v>
+      </c>
+      <c r="L8" s="53">
+        <v>0</v>
+      </c>
+      <c r="M8" s="63">
+        <v>0</v>
+      </c>
+      <c r="N8" s="52">
+        <v>0</v>
+      </c>
+      <c r="O8" s="52">
+        <v>0</v>
+      </c>
+      <c r="P8" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="52">
+        <v>0</v>
+      </c>
+      <c r="R8" s="52">
+        <v>0</v>
+      </c>
+      <c r="S8" s="52">
+        <v>0</v>
+      </c>
+      <c r="T8" s="53">
+        <v>0</v>
+      </c>
+      <c r="U8" s="76">
+        <v>0</v>
+      </c>
+      <c r="V8" s="59">
+        <v>0</v>
+      </c>
+      <c r="W8" s="59">
+        <v>0</v>
+      </c>
+      <c r="X8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD8" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE8" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="13">
+        <v>68</v>
+      </c>
+      <c r="D9" s="75" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E9" s="52">
+        <v>0</v>
+      </c>
+      <c r="F9" s="52">
+        <v>0</v>
+      </c>
+      <c r="G9" s="52">
+        <v>0</v>
+      </c>
+      <c r="H9" s="52">
+        <v>0</v>
+      </c>
+      <c r="I9" s="52">
+        <v>0</v>
+      </c>
+      <c r="J9" s="52">
+        <v>0</v>
+      </c>
+      <c r="K9" s="52">
+        <v>0</v>
+      </c>
+      <c r="L9" s="53">
+        <v>0</v>
+      </c>
+      <c r="M9" s="63">
+        <v>0</v>
+      </c>
+      <c r="N9" s="52">
+        <v>0</v>
+      </c>
+      <c r="O9" s="52">
+        <v>0</v>
+      </c>
+      <c r="P9" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="52">
+        <v>0</v>
+      </c>
+      <c r="R9" s="52">
+        <v>0</v>
+      </c>
+      <c r="S9" s="52">
+        <v>0</v>
+      </c>
+      <c r="T9" s="53">
+        <v>0</v>
+      </c>
+      <c r="U9" s="76">
+        <v>0</v>
+      </c>
+      <c r="V9" s="59">
+        <v>0</v>
+      </c>
+      <c r="W9" s="59">
+        <v>0</v>
+      </c>
+      <c r="X9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD9" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE9" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF9" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:36" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="12">
+        <v>66</v>
+      </c>
+      <c r="D15" s="22" t="str">
+        <f t="shared" ref="D15" si="1">"0x00"&amp;TEXT(DEC2HEX(L15+2*K15+4*J15+8*I15+16*H15+32*G15+64*F15+128*E15,2),"00")&amp;TEXT(DEC2HEX(T15+2*S15+4*R15+8*Q15+16*P15+32*O15+64*N15+128*M15,2),"00")&amp;TEXT(DEC2HEX(AB15+2*AA15+4*Z15+8*Y15+16*X15+32*W15+64*V15+128*U15,2),"00")</f>
+        <v>0x001F8E0B</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0</v>
+      </c>
+      <c r="F15" s="37">
+        <v>0</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
+      <c r="H15" s="30">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="19">
+        <v>0</v>
+      </c>
+      <c r="O15" s="19">
+        <v>0</v>
+      </c>
+      <c r="P15" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>1</v>
+      </c>
+      <c r="R15" s="8">
+        <v>1</v>
+      </c>
+      <c r="S15" s="8">
+        <v>1</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="19">
+        <v>0</v>
+      </c>
+      <c r="V15" s="8">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="41">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="42">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="39">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="40">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="107" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="4">
+        <v>31</v>
+      </c>
+      <c r="F16" s="4">
+        <v>30</v>
+      </c>
+      <c r="G16" s="4">
+        <v>29</v>
+      </c>
+      <c r="H16" s="4">
+        <v>28</v>
+      </c>
+      <c r="I16" s="4">
+        <v>27</v>
+      </c>
+      <c r="J16" s="4">
+        <v>26</v>
+      </c>
+      <c r="K16" s="4">
+        <v>25</v>
+      </c>
+      <c r="L16" s="4">
+        <v>24</v>
+      </c>
+      <c r="M16" s="4">
+        <v>23</v>
+      </c>
+      <c r="N16" s="4">
+        <v>22</v>
+      </c>
+      <c r="O16" s="4">
+        <v>21</v>
+      </c>
+      <c r="P16" s="4">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>19</v>
+      </c>
+      <c r="R16" s="4">
+        <v>18</v>
+      </c>
+      <c r="S16" s="4">
+        <v>17</v>
+      </c>
+      <c r="T16" s="4">
+        <v>16</v>
+      </c>
+      <c r="U16" s="4">
+        <v>15</v>
+      </c>
+      <c r="V16" s="4">
+        <v>14</v>
+      </c>
+      <c r="W16" s="4">
+        <v>13</v>
+      </c>
+      <c r="X16" s="4">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>11</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>9</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>8</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>7</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>6</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>5</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="11">
+        <v>73</v>
+      </c>
+      <c r="D17" s="22" t="str">
+        <f>"0x"&amp;TEXT(DEC2HEX(L17+2*K17+4*J17+8*I17+16*H17+32*G17+64*F17+128*E17,2),"00")&amp;TEXT(DEC2HEX(T17+2*S17+4*R17+8*Q17+16*P17+32*O17+64*N17+128*M17,2),"00")&amp;TEXT(DEC2HEX(AB17+2*AA17+4*Z17+8*Y17+16*X17+32*W17+64*V17+128*U17,2),"00")&amp;TEXT(DEC2HEX(AJ17+2*AI17+4*AH17+8*AG17+16*AF17+32*AE17+64*AD17+128*AC17,2),"00")</f>
+        <v>0x80800000</v>
+      </c>
+      <c r="E17" s="46">
+        <v>1</v>
+      </c>
+      <c r="F17" s="46">
+        <v>0</v>
+      </c>
+      <c r="G17" s="46">
+        <v>0</v>
+      </c>
+      <c r="H17" s="46">
+        <v>0</v>
+      </c>
+      <c r="I17" s="46">
+        <v>0</v>
+      </c>
+      <c r="J17" s="27">
+        <v>0</v>
+      </c>
+      <c r="K17" s="28">
+        <v>0</v>
+      </c>
+      <c r="L17" s="29">
+        <v>0</v>
+      </c>
+      <c r="M17" s="44">
+        <v>1</v>
+      </c>
+      <c r="N17" s="46">
+        <v>0</v>
+      </c>
+      <c r="O17" s="46">
+        <v>0</v>
+      </c>
+      <c r="P17" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="46">
+        <v>0</v>
+      </c>
+      <c r="R17" s="46">
+        <v>0</v>
+      </c>
+      <c r="S17" s="46">
+        <v>0</v>
+      </c>
+      <c r="T17" s="46">
+        <v>0</v>
+      </c>
+      <c r="U17" s="46">
+        <v>0</v>
+      </c>
+      <c r="V17" s="46">
+        <v>0</v>
+      </c>
+      <c r="W17" s="46">
+        <v>0</v>
+      </c>
+      <c r="X17" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="46">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="46">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="46">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y4" sqref="A1:AG10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="2.5703125" customWidth="1"/>
+    <col min="21" max="28" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="52">
+        <v>23</v>
+      </c>
+      <c r="F1" s="52">
+        <v>22</v>
+      </c>
+      <c r="G1" s="52">
+        <v>21</v>
+      </c>
+      <c r="H1" s="52">
+        <v>20</v>
+      </c>
+      <c r="I1" s="52">
+        <v>19</v>
+      </c>
+      <c r="J1" s="52">
+        <v>18</v>
+      </c>
+      <c r="K1" s="52">
+        <v>17</v>
+      </c>
+      <c r="L1" s="53">
+        <v>16</v>
+      </c>
+      <c r="M1" s="63">
+        <v>15</v>
+      </c>
+      <c r="N1" s="52">
+        <v>14</v>
+      </c>
+      <c r="O1" s="52">
+        <v>13</v>
+      </c>
+      <c r="P1" s="52">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="52">
+        <v>11</v>
+      </c>
+      <c r="R1" s="52">
+        <v>10</v>
+      </c>
+      <c r="S1" s="52">
+        <v>9</v>
+      </c>
+      <c r="T1" s="53">
+        <v>8</v>
+      </c>
+      <c r="U1" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="13">
+        <v>62</v>
+      </c>
+      <c r="D2" s="82" t="str">
+        <f>"0x00"&amp;TEXT(DEC2HEX(L2+2*K2+4*J2+8*I2+16*H2+32*G2+64*F2+128*E2,2),"00")&amp;TEXT(DEC2HEX(T2+2*S2+4*R2+8*Q2+16*P2+32*O2+64*N2+128*M2,2),"00")&amp;TEXT(DEC2HEX(AB2+2*AA2+4*Z2+8*Y2+16*X2+32*W2+64*V2+128*U2,2),"00")</f>
+        <v>0x00A0000A</v>
+      </c>
+      <c r="E2" s="83">
+        <v>1</v>
+      </c>
+      <c r="F2" s="83">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34">
+        <v>1</v>
+      </c>
+      <c r="H2" s="84">
+        <v>0</v>
+      </c>
+      <c r="I2" s="85">
+        <v>0</v>
+      </c>
+      <c r="J2" s="85">
+        <v>0</v>
+      </c>
+      <c r="K2" s="85">
+        <v>0</v>
+      </c>
+      <c r="L2" s="86">
+        <v>0</v>
+      </c>
+      <c r="M2" s="87">
+        <v>0</v>
+      </c>
+      <c r="N2" s="100">
+        <v>0</v>
+      </c>
+      <c r="O2" s="83">
+        <v>0</v>
+      </c>
+      <c r="P2" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="85">
+        <v>0</v>
+      </c>
+      <c r="R2" s="85">
+        <v>0</v>
+      </c>
+      <c r="S2" s="52">
+        <v>0</v>
+      </c>
+      <c r="T2" s="89">
+        <v>0</v>
+      </c>
+      <c r="U2" s="88">
+        <v>0</v>
+      </c>
+      <c r="V2" s="83">
+        <v>0</v>
+      </c>
+      <c r="W2" s="83">
+        <v>0</v>
+      </c>
+      <c r="X2" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="59">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="59">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="77">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="12">
+        <v>66</v>
+      </c>
+      <c r="D3" s="82" t="str">
+        <f t="shared" ref="D3:D10" si="0">"0x00"&amp;TEXT(DEC2HEX(L3+2*K3+4*J3+8*I3+16*H3+32*G3+64*F3+128*E3,2),"00")&amp;TEXT(DEC2HEX(T3+2*S3+4*R3+8*Q3+16*P3+32*O3+64*N3+128*M3,2),"00")&amp;TEXT(DEC2HEX(AB3+2*AA3+4*Z3+8*Y3+16*X3+32*W3+64*V3+128*U3,2),"00")</f>
+        <v>0x001F8E08</v>
+      </c>
+      <c r="E3" s="72">
+        <v>0</v>
+      </c>
+      <c r="F3" s="72">
+        <v>0</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0</v>
+      </c>
+      <c r="H3" s="84">
+        <v>1</v>
+      </c>
+      <c r="I3" s="85">
+        <v>1</v>
+      </c>
+      <c r="J3" s="85">
+        <v>1</v>
+      </c>
+      <c r="K3" s="85">
+        <v>1</v>
+      </c>
+      <c r="L3" s="86">
+        <v>1</v>
+      </c>
+      <c r="M3" s="90">
+        <v>1</v>
+      </c>
+      <c r="N3" s="59">
+        <v>0</v>
+      </c>
+      <c r="O3" s="59">
+        <v>0</v>
+      </c>
+      <c r="P3" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="59">
+        <v>1</v>
+      </c>
+      <c r="R3" s="59">
+        <v>1</v>
+      </c>
+      <c r="S3" s="59">
+        <v>1</v>
+      </c>
+      <c r="T3" s="86">
+        <v>0</v>
+      </c>
+      <c r="U3" s="76">
+        <v>0</v>
+      </c>
+      <c r="V3" s="59">
+        <v>0</v>
+      </c>
+      <c r="W3" s="94">
+        <v>0</v>
+      </c>
+      <c r="X3" s="66">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="67">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="67">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="13">
+        <v>58</v>
+      </c>
+      <c r="D4" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00A004CE</v>
+      </c>
+      <c r="E4" s="72">
+        <v>1</v>
+      </c>
+      <c r="F4" s="72">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="84">
+        <v>0</v>
+      </c>
+      <c r="I4" s="85">
+        <v>0</v>
+      </c>
+      <c r="J4" s="85">
+        <v>0</v>
+      </c>
+      <c r="K4" s="85">
+        <v>0</v>
+      </c>
+      <c r="L4" s="86">
+        <v>0</v>
+      </c>
+      <c r="M4" s="90">
+        <v>0</v>
+      </c>
+      <c r="N4" s="85">
+        <v>0</v>
+      </c>
+      <c r="O4" s="85">
+        <v>0</v>
+      </c>
+      <c r="P4" s="85">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="96">
+        <v>0</v>
+      </c>
+      <c r="R4" s="66">
+        <v>1</v>
+      </c>
+      <c r="S4" s="52">
+        <v>0</v>
+      </c>
+      <c r="T4" s="53">
+        <v>0</v>
+      </c>
+      <c r="U4" s="63">
+        <v>1</v>
+      </c>
+      <c r="V4" s="59">
+        <v>1</v>
+      </c>
+      <c r="W4" s="59">
+        <v>0</v>
+      </c>
+      <c r="X4" s="52">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="58">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="52">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="53">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD4" s="79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="13">
+        <v>60</v>
+      </c>
+      <c r="D5" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00002001</v>
+      </c>
+      <c r="E5" s="93">
+        <v>0</v>
+      </c>
+      <c r="F5" s="94">
+        <v>0</v>
+      </c>
+      <c r="G5" s="94">
+        <v>0</v>
+      </c>
+      <c r="H5" s="85">
+        <v>0</v>
+      </c>
+      <c r="I5" s="85">
+        <v>0</v>
+      </c>
+      <c r="J5" s="85">
+        <v>0</v>
+      </c>
+      <c r="K5" s="85">
+        <v>0</v>
+      </c>
+      <c r="L5" s="53">
+        <v>0</v>
+      </c>
+      <c r="M5" s="63">
+        <v>0</v>
+      </c>
+      <c r="N5" s="52">
+        <v>0</v>
+      </c>
+      <c r="O5" s="59">
+        <v>1</v>
+      </c>
+      <c r="P5" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <v>0</v>
+      </c>
+      <c r="S5" s="28">
+        <v>0</v>
+      </c>
+      <c r="T5" s="29">
+        <v>0</v>
+      </c>
+      <c r="U5" s="76">
+        <v>0</v>
+      </c>
+      <c r="V5" s="88">
+        <v>0</v>
+      </c>
+      <c r="W5" s="34">
+        <v>0</v>
+      </c>
+      <c r="X5" s="98">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="99">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="79" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="13">
+        <v>61</v>
+      </c>
+      <c r="D6" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000E01</v>
+      </c>
+      <c r="E6" s="84">
+        <v>0</v>
+      </c>
+      <c r="F6" s="85">
+        <v>0</v>
+      </c>
+      <c r="G6" s="85">
+        <v>0</v>
+      </c>
+      <c r="H6" s="85">
+        <v>0</v>
+      </c>
+      <c r="I6" s="85">
+        <v>0</v>
+      </c>
+      <c r="J6" s="85">
+        <v>0</v>
+      </c>
+      <c r="K6" s="85">
+        <v>0</v>
+      </c>
+      <c r="L6" s="86">
+        <v>0</v>
+      </c>
+      <c r="M6" s="90">
+        <v>0</v>
+      </c>
+      <c r="N6" s="85">
+        <v>0</v>
+      </c>
+      <c r="O6" s="85">
+        <v>0</v>
+      </c>
+      <c r="P6" s="85">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="59">
+        <v>1</v>
+      </c>
+      <c r="R6" s="59">
+        <v>1</v>
+      </c>
+      <c r="S6" s="59">
+        <v>1</v>
+      </c>
+      <c r="T6" s="97">
+        <v>0</v>
+      </c>
+      <c r="U6" s="95">
+        <v>0</v>
+      </c>
+      <c r="V6" s="88">
+        <v>0</v>
+      </c>
+      <c r="W6" s="34">
+        <v>0</v>
+      </c>
+      <c r="X6" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="79" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13">
+        <v>64</v>
+      </c>
+      <c r="D7" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000030</v>
+      </c>
+      <c r="E7" s="102">
+        <v>0</v>
+      </c>
+      <c r="F7" s="102">
+        <v>0</v>
+      </c>
+      <c r="G7" s="102">
+        <v>0</v>
+      </c>
+      <c r="H7" s="102">
+        <v>0</v>
+      </c>
+      <c r="I7" s="102">
+        <v>0</v>
+      </c>
+      <c r="J7" s="102">
+        <v>0</v>
+      </c>
+      <c r="K7" s="102">
+        <v>0</v>
+      </c>
+      <c r="L7" s="103">
+        <v>0</v>
+      </c>
+      <c r="M7" s="102">
+        <v>0</v>
+      </c>
+      <c r="N7" s="102">
+        <v>0</v>
+      </c>
+      <c r="O7" s="102">
+        <v>0</v>
+      </c>
+      <c r="P7" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="102">
+        <v>0</v>
+      </c>
+      <c r="R7" s="102">
+        <v>0</v>
+      </c>
+      <c r="S7" s="102">
+        <v>0</v>
+      </c>
+      <c r="T7" s="103">
+        <v>0</v>
+      </c>
+      <c r="U7" s="59">
+        <v>0</v>
+      </c>
+      <c r="V7" s="58">
+        <v>0</v>
+      </c>
+      <c r="W7" s="59">
+        <v>1</v>
+      </c>
+      <c r="X7" s="59">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="13">
+        <v>68</v>
+      </c>
+      <c r="D8" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E8" s="102">
+        <v>0</v>
+      </c>
+      <c r="F8" s="102">
+        <v>0</v>
+      </c>
+      <c r="G8" s="102">
+        <v>0</v>
+      </c>
+      <c r="H8" s="102">
+        <v>0</v>
+      </c>
+      <c r="I8" s="102">
+        <v>0</v>
+      </c>
+      <c r="J8" s="102">
+        <v>0</v>
+      </c>
+      <c r="K8" s="102">
+        <v>0</v>
+      </c>
+      <c r="L8" s="103">
+        <v>0</v>
+      </c>
+      <c r="M8" s="104">
+        <v>0</v>
+      </c>
+      <c r="N8" s="102">
+        <v>0</v>
+      </c>
+      <c r="O8" s="102">
+        <v>0</v>
+      </c>
+      <c r="P8" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="102">
+        <v>0</v>
+      </c>
+      <c r="R8" s="102">
+        <v>0</v>
+      </c>
+      <c r="S8" s="102">
+        <v>0</v>
+      </c>
+      <c r="T8" s="103">
+        <v>0</v>
+      </c>
+      <c r="U8" s="76">
+        <v>0</v>
+      </c>
+      <c r="V8" s="59">
+        <v>0</v>
+      </c>
+      <c r="W8" s="59">
+        <v>0</v>
+      </c>
+      <c r="X8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD8" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE8" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="13">
+        <v>68</v>
+      </c>
+      <c r="D9" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E9" s="102">
+        <v>0</v>
+      </c>
+      <c r="F9" s="102">
+        <v>0</v>
+      </c>
+      <c r="G9" s="102">
+        <v>0</v>
+      </c>
+      <c r="H9" s="102">
+        <v>0</v>
+      </c>
+      <c r="I9" s="102">
+        <v>0</v>
+      </c>
+      <c r="J9" s="102">
+        <v>0</v>
+      </c>
+      <c r="K9" s="102">
+        <v>0</v>
+      </c>
+      <c r="L9" s="103">
+        <v>0</v>
+      </c>
+      <c r="M9" s="104">
+        <v>0</v>
+      </c>
+      <c r="N9" s="102">
+        <v>0</v>
+      </c>
+      <c r="O9" s="102">
+        <v>0</v>
+      </c>
+      <c r="P9" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="102">
+        <v>0</v>
+      </c>
+      <c r="R9" s="102">
+        <v>0</v>
+      </c>
+      <c r="S9" s="102">
+        <v>0</v>
+      </c>
+      <c r="T9" s="103">
+        <v>0</v>
+      </c>
+      <c r="U9" s="76">
+        <v>0</v>
+      </c>
+      <c r="V9" s="59">
+        <v>0</v>
+      </c>
+      <c r="W9" s="59">
+        <v>0</v>
+      </c>
+      <c r="X9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD9" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE9" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF9" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG9" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <f>(B12*1.8*2)/(1.4*65536)</f>
+        <v>1.883370535714286E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>36</v>
+      </c>
+      <c r="C13" s="79">
+        <f>(B13*1.8)/(1.4*65536)</f>
+        <v>7.0626395089285713E-4</v>
+      </c>
+      <c r="D13" s="79">
+        <f>1.8/1.4/65536</f>
+        <v>1.9618443080357144E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" s="79">
+        <f>(B14*1.8)/(1.4*65536)</f>
+        <v>3.1389508928571431E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="80"/>
+    <col min="4" max="4" width="12" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="18" width="3" style="80" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="2.5703125" style="80" customWidth="1"/>
+    <col min="21" max="28" width="3.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" style="80" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" style="80" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="52">
+        <v>23</v>
+      </c>
+      <c r="F1" s="52">
+        <v>22</v>
+      </c>
+      <c r="G1" s="52">
+        <v>21</v>
+      </c>
+      <c r="H1" s="52">
+        <v>20</v>
+      </c>
+      <c r="I1" s="52">
+        <v>19</v>
+      </c>
+      <c r="J1" s="52">
+        <v>18</v>
+      </c>
+      <c r="K1" s="52">
+        <v>17</v>
+      </c>
+      <c r="L1" s="53">
+        <v>16</v>
+      </c>
+      <c r="M1" s="63">
+        <v>15</v>
+      </c>
+      <c r="N1" s="52">
+        <v>14</v>
+      </c>
+      <c r="O1" s="52">
+        <v>13</v>
+      </c>
+      <c r="P1" s="52">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="52">
+        <v>11</v>
+      </c>
+      <c r="R1" s="52">
+        <v>10</v>
+      </c>
+      <c r="S1" s="52">
+        <v>9</v>
+      </c>
+      <c r="T1" s="53">
+        <v>8</v>
+      </c>
+      <c r="U1" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="13">
+        <v>62</v>
+      </c>
+      <c r="D2" s="82" t="str">
+        <f>"0x00"&amp;TEXT(DEC2HEX(L2+2*K2+4*J2+8*I2+16*H2+32*G2+64*F2+128*E2,2),"00")&amp;TEXT(DEC2HEX(T2+2*S2+4*R2+8*Q2+16*P2+32*O2+64*N2+128*M2,2),"00")&amp;TEXT(DEC2HEX(AB2+2*AA2+4*Z2+8*Y2+16*X2+32*W2+64*V2+128*U2,2),"00")</f>
+        <v>0x00A0000A</v>
+      </c>
+      <c r="E2" s="83">
+        <v>1</v>
+      </c>
+      <c r="F2" s="83">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34">
+        <v>1</v>
+      </c>
+      <c r="H2" s="84">
+        <v>0</v>
+      </c>
+      <c r="I2" s="85">
+        <v>0</v>
+      </c>
+      <c r="J2" s="85">
+        <v>0</v>
+      </c>
+      <c r="K2" s="85">
+        <v>0</v>
+      </c>
+      <c r="L2" s="86">
+        <v>0</v>
+      </c>
+      <c r="M2" s="87">
+        <v>0</v>
+      </c>
+      <c r="N2" s="100">
+        <v>0</v>
+      </c>
+      <c r="O2" s="83">
+        <v>0</v>
+      </c>
+      <c r="P2" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="85">
+        <v>0</v>
+      </c>
+      <c r="R2" s="85">
+        <v>0</v>
+      </c>
+      <c r="S2" s="52">
+        <v>0</v>
+      </c>
+      <c r="T2" s="89">
+        <v>0</v>
+      </c>
+      <c r="U2" s="88">
+        <v>0</v>
+      </c>
+      <c r="V2" s="83">
+        <v>0</v>
+      </c>
+      <c r="W2" s="83">
+        <v>0</v>
+      </c>
+      <c r="X2" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="59">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="59">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="77">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="12">
+        <v>66</v>
+      </c>
+      <c r="D3" s="82" t="str">
+        <f t="shared" ref="D3:D10" si="0">"0x00"&amp;TEXT(DEC2HEX(L3+2*K3+4*J3+8*I3+16*H3+32*G3+64*F3+128*E3,2),"00")&amp;TEXT(DEC2HEX(T3+2*S3+4*R3+8*Q3+16*P3+32*O3+64*N3+128*M3,2),"00")&amp;TEXT(DEC2HEX(AB3+2*AA3+4*Z3+8*Y3+16*X3+32*W3+64*V3+128*U3,2),"00")</f>
+        <v>0x001F8E03</v>
+      </c>
+      <c r="E3" s="72">
+        <v>0</v>
+      </c>
+      <c r="F3" s="72">
+        <v>0</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0</v>
+      </c>
+      <c r="H3" s="84">
+        <v>1</v>
+      </c>
+      <c r="I3" s="85">
+        <v>1</v>
+      </c>
+      <c r="J3" s="85">
+        <v>1</v>
+      </c>
+      <c r="K3" s="85">
+        <v>1</v>
+      </c>
+      <c r="L3" s="86">
+        <v>1</v>
+      </c>
+      <c r="M3" s="90">
+        <v>1</v>
+      </c>
+      <c r="N3" s="59">
+        <v>0</v>
+      </c>
+      <c r="O3" s="59">
+        <v>0</v>
+      </c>
+      <c r="P3" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="59">
+        <v>1</v>
+      </c>
+      <c r="R3" s="59">
+        <v>1</v>
+      </c>
+      <c r="S3" s="59">
+        <v>1</v>
+      </c>
+      <c r="T3" s="86">
+        <v>0</v>
+      </c>
+      <c r="U3" s="76">
+        <v>0</v>
+      </c>
+      <c r="V3" s="59">
+        <v>0</v>
+      </c>
+      <c r="W3" s="94">
+        <v>0</v>
+      </c>
+      <c r="X3" s="66">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="67">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="67">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="91">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="92">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="80" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="13">
+        <v>58</v>
+      </c>
+      <c r="D4" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00A004C6</v>
+      </c>
+      <c r="E4" s="72">
+        <v>1</v>
+      </c>
+      <c r="F4" s="72">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="84">
+        <v>0</v>
+      </c>
+      <c r="I4" s="85">
+        <v>0</v>
+      </c>
+      <c r="J4" s="85">
+        <v>0</v>
+      </c>
+      <c r="K4" s="85">
+        <v>0</v>
+      </c>
+      <c r="L4" s="86">
+        <v>0</v>
+      </c>
+      <c r="M4" s="90">
+        <v>0</v>
+      </c>
+      <c r="N4" s="85">
+        <v>0</v>
+      </c>
+      <c r="O4" s="85">
+        <v>0</v>
+      </c>
+      <c r="P4" s="85">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="96">
+        <v>0</v>
+      </c>
+      <c r="R4" s="66">
+        <v>1</v>
+      </c>
+      <c r="S4" s="52">
+        <v>0</v>
+      </c>
+      <c r="T4" s="53">
+        <v>0</v>
+      </c>
+      <c r="U4" s="63">
+        <v>1</v>
+      </c>
+      <c r="V4" s="59">
+        <v>1</v>
+      </c>
+      <c r="W4" s="59">
+        <v>0</v>
+      </c>
+      <c r="X4" s="52">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="58">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="52">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="53">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD4" s="80" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="13">
+        <v>60</v>
+      </c>
+      <c r="D5" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00002001</v>
+      </c>
+      <c r="E5" s="93">
+        <v>0</v>
+      </c>
+      <c r="F5" s="94">
+        <v>0</v>
+      </c>
+      <c r="G5" s="94">
+        <v>0</v>
+      </c>
+      <c r="H5" s="85">
+        <v>0</v>
+      </c>
+      <c r="I5" s="85">
+        <v>0</v>
+      </c>
+      <c r="J5" s="85">
+        <v>0</v>
+      </c>
+      <c r="K5" s="85">
+        <v>0</v>
+      </c>
+      <c r="L5" s="53">
+        <v>0</v>
+      </c>
+      <c r="M5" s="63">
+        <v>0</v>
+      </c>
+      <c r="N5" s="52">
+        <v>0</v>
+      </c>
+      <c r="O5" s="59">
+        <v>1</v>
+      </c>
+      <c r="P5" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <v>0</v>
+      </c>
+      <c r="S5" s="28">
+        <v>0</v>
+      </c>
+      <c r="T5" s="29">
+        <v>0</v>
+      </c>
+      <c r="U5" s="76">
+        <v>0</v>
+      </c>
+      <c r="V5" s="88">
+        <v>0</v>
+      </c>
+      <c r="W5" s="34">
+        <v>0</v>
+      </c>
+      <c r="X5" s="98">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="99">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="13">
+        <v>61</v>
+      </c>
+      <c r="D6" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E6" s="84">
+        <v>0</v>
+      </c>
+      <c r="F6" s="85">
+        <v>0</v>
+      </c>
+      <c r="G6" s="85">
+        <v>0</v>
+      </c>
+      <c r="H6" s="85">
+        <v>0</v>
+      </c>
+      <c r="I6" s="85">
+        <v>0</v>
+      </c>
+      <c r="J6" s="85">
+        <v>0</v>
+      </c>
+      <c r="K6" s="85">
+        <v>0</v>
+      </c>
+      <c r="L6" s="86">
+        <v>0</v>
+      </c>
+      <c r="M6" s="90">
+        <v>0</v>
+      </c>
+      <c r="N6" s="85">
+        <v>0</v>
+      </c>
+      <c r="O6" s="85">
+        <v>0</v>
+      </c>
+      <c r="P6" s="85">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="59">
+        <v>0</v>
+      </c>
+      <c r="R6" s="59">
+        <v>0</v>
+      </c>
+      <c r="S6" s="59">
+        <v>0</v>
+      </c>
+      <c r="T6" s="97">
+        <v>0</v>
+      </c>
+      <c r="U6" s="95">
+        <v>0</v>
+      </c>
+      <c r="V6" s="88">
+        <v>0</v>
+      </c>
+      <c r="W6" s="34">
+        <v>0</v>
+      </c>
+      <c r="X6" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="13">
+        <v>64</v>
+      </c>
+      <c r="D7" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E7" s="102">
+        <v>0</v>
+      </c>
+      <c r="F7" s="102">
+        <v>0</v>
+      </c>
+      <c r="G7" s="102">
+        <v>0</v>
+      </c>
+      <c r="H7" s="102">
+        <v>0</v>
+      </c>
+      <c r="I7" s="102">
+        <v>0</v>
+      </c>
+      <c r="J7" s="102">
+        <v>0</v>
+      </c>
+      <c r="K7" s="102">
+        <v>0</v>
+      </c>
+      <c r="L7" s="103">
+        <v>0</v>
+      </c>
+      <c r="M7" s="102">
+        <v>0</v>
+      </c>
+      <c r="N7" s="102">
+        <v>0</v>
+      </c>
+      <c r="O7" s="102">
+        <v>0</v>
+      </c>
+      <c r="P7" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="102">
+        <v>0</v>
+      </c>
+      <c r="R7" s="102">
+        <v>0</v>
+      </c>
+      <c r="S7" s="102">
+        <v>0</v>
+      </c>
+      <c r="T7" s="103">
+        <v>0</v>
+      </c>
+      <c r="U7" s="59">
+        <v>0</v>
+      </c>
+      <c r="V7" s="58">
+        <v>0</v>
+      </c>
+      <c r="W7" s="59">
+        <v>0</v>
+      </c>
+      <c r="X7" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="13">
+        <v>68</v>
+      </c>
+      <c r="D8" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E8" s="102">
+        <v>0</v>
+      </c>
+      <c r="F8" s="102">
+        <v>0</v>
+      </c>
+      <c r="G8" s="102">
+        <v>0</v>
+      </c>
+      <c r="H8" s="102">
+        <v>0</v>
+      </c>
+      <c r="I8" s="102">
+        <v>0</v>
+      </c>
+      <c r="J8" s="102">
+        <v>0</v>
+      </c>
+      <c r="K8" s="102">
+        <v>0</v>
+      </c>
+      <c r="L8" s="103">
+        <v>0</v>
+      </c>
+      <c r="M8" s="104">
+        <v>0</v>
+      </c>
+      <c r="N8" s="102">
+        <v>0</v>
+      </c>
+      <c r="O8" s="102">
+        <v>0</v>
+      </c>
+      <c r="P8" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="102">
+        <v>0</v>
+      </c>
+      <c r="R8" s="102">
+        <v>0</v>
+      </c>
+      <c r="S8" s="102">
+        <v>0</v>
+      </c>
+      <c r="T8" s="103">
+        <v>0</v>
+      </c>
+      <c r="U8" s="76">
+        <v>0</v>
+      </c>
+      <c r="V8" s="59">
+        <v>0</v>
+      </c>
+      <c r="W8" s="59">
+        <v>0</v>
+      </c>
+      <c r="X8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD8" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE8" s="80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="13">
+        <v>68</v>
+      </c>
+      <c r="D9" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+      <c r="E9" s="102">
+        <v>0</v>
+      </c>
+      <c r="F9" s="102">
+        <v>0</v>
+      </c>
+      <c r="G9" s="102">
+        <v>0</v>
+      </c>
+      <c r="H9" s="102">
+        <v>0</v>
+      </c>
+      <c r="I9" s="102">
+        <v>0</v>
+      </c>
+      <c r="J9" s="102">
+        <v>0</v>
+      </c>
+      <c r="K9" s="102">
+        <v>0</v>
+      </c>
+      <c r="L9" s="103">
+        <v>0</v>
+      </c>
+      <c r="M9" s="104">
+        <v>0</v>
+      </c>
+      <c r="N9" s="102">
+        <v>0</v>
+      </c>
+      <c r="O9" s="102">
+        <v>0</v>
+      </c>
+      <c r="P9" s="102">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="102">
+        <v>0</v>
+      </c>
+      <c r="R9" s="102">
+        <v>0</v>
+      </c>
+      <c r="S9" s="102">
+        <v>0</v>
+      </c>
+      <c r="T9" s="103">
+        <v>0</v>
+      </c>
+      <c r="U9" s="76">
+        <v>0</v>
+      </c>
+      <c r="V9" s="59">
+        <v>0</v>
+      </c>
+      <c r="W9" s="59">
+        <v>0</v>
+      </c>
+      <c r="X9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="77">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD9" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE9" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF9" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG9" s="80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0x00000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="80">
+        <v>48</v>
+      </c>
+      <c r="C12" s="80">
+        <f>(B12*1.8*2)/(1.4*65536)</f>
+        <v>1.883370535714286E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="80">
+        <v>36</v>
+      </c>
+      <c r="C13" s="80">
+        <f>(B13*1.8)/(1.4*65536)</f>
+        <v>7.0626395089285713E-4</v>
+      </c>
+      <c r="D13" s="80">
+        <f>1.8/1.4/65536</f>
+        <v>1.9618443080357144E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="80">
+        <v>16</v>
+      </c>
+      <c r="C14" s="80">
+        <f>(B14*1.8)/(1.4*65536)</f>
+        <v>3.1389508928571431E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>